<commit_message>
Casos de prueba finales.
53 de 55 casos de prueba certificados. Orgullo
</commit_message>
<xml_diff>
--- a/Documentación/Casos Prueba_Pet Saviors.xlsx
+++ b/Documentación/Casos Prueba_Pet Saviors.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="176">
   <si>
     <t>Caso 01</t>
   </si>
@@ -271,9 +271,6 @@
   </si>
   <si>
     <t>Caso 34</t>
-  </si>
-  <si>
-    <t>En la piedra</t>
   </si>
   <si>
     <t xml:space="preserve">Entrar a la ventana "Mascotas". </t>
@@ -1217,7 +1214,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1225,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:G72"/>
+  <dimension ref="A4:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1260,10 +1257,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
         <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
@@ -1281,7 +1278,7 @@
         <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>41</v>
@@ -1290,7 +1287,7 @@
         <v>41</v>
       </c>
       <c r="G7" s="6">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1330,7 +1327,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1338,10 +1335,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>41</v>
@@ -1350,7 +1347,7 @@
         <v>52</v>
       </c>
       <c r="G10" s="6">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1358,10 +1355,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>41</v>
@@ -1375,7 +1372,7 @@
         <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>41</v>
@@ -1384,7 +1381,7 @@
         <v>64</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1392,10 +1389,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>41</v>
@@ -1406,10 +1403,10 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>41</v>
@@ -1420,10 +1417,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>41</v>
@@ -1434,7 +1431,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>66</v>
@@ -1448,10 +1445,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>41</v>
@@ -1464,10 +1461,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>41</v>
@@ -1480,10 +1477,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
@@ -1496,10 +1493,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>41</v>
@@ -1510,10 +1507,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>41</v>
@@ -1524,10 +1521,10 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>41</v>
@@ -1538,10 +1535,10 @@
         <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>41</v>
@@ -1552,10 +1549,10 @@
         <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>41</v>
@@ -1566,10 +1563,10 @@
         <v>69</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>106</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>41</v>
@@ -1580,10 +1577,10 @@
         <v>70</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>41</v>
@@ -1594,10 +1591,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>41</v>
@@ -1608,10 +1605,10 @@
         <v>20</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>41</v>
@@ -1622,10 +1619,10 @@
         <v>21</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>41</v>
@@ -1636,10 +1633,10 @@
         <v>22</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>41</v>
@@ -1650,10 +1647,10 @@
         <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>41</v>
@@ -1664,10 +1661,10 @@
         <v>24</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>41</v>
@@ -1678,10 +1675,10 @@
         <v>25</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>41</v>
@@ -1692,10 +1689,10 @@
         <v>26</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>41</v>
@@ -1706,10 +1703,10 @@
         <v>27</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>41</v>
@@ -1720,10 +1717,10 @@
         <v>31</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>41</v>
@@ -1734,13 +1731,13 @@
         <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1748,10 +1745,10 @@
         <v>33</v>
       </c>
       <c r="B38" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>41</v>
@@ -1762,10 +1759,10 @@
         <v>71</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>41</v>
@@ -1776,10 +1773,10 @@
         <v>34</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>41</v>
@@ -1790,10 +1787,10 @@
         <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>41</v>
@@ -1804,10 +1801,10 @@
         <v>36</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>41</v>
@@ -1818,10 +1815,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>41</v>
@@ -1832,10 +1829,10 @@
         <v>38</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>41</v>
@@ -1846,10 +1843,10 @@
         <v>39</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>41</v>
@@ -1860,10 +1857,10 @@
         <v>42</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>41</v>
@@ -1874,10 +1871,10 @@
         <v>43</v>
       </c>
       <c r="B47" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>41</v>
@@ -1888,10 +1885,10 @@
         <v>44</v>
       </c>
       <c r="B48" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>41</v>
@@ -1902,13 +1899,13 @@
         <v>45</v>
       </c>
       <c r="B49" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>149</v>
-      </c>
       <c r="D49" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1916,13 +1913,13 @@
         <v>46</v>
       </c>
       <c r="B50" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="D50" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1930,13 +1927,13 @@
         <v>47</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1944,10 +1941,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>41</v>
@@ -1957,14 +1954,14 @@
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>142</v>
+      <c r="B53" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1972,10 +1969,10 @@
         <v>50</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>41</v>
@@ -1986,90 +1983,90 @@
         <v>51</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="1"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>169</v>
+        <v>56</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1"/>
@@ -2085,40 +2082,25 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1"/>
-      <c r="B64" s="9"/>
+      <c r="B64" s="10"/>
       <c r="C64" s="9"/>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:3">
       <c r="A65" s="1"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:3">
       <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:4">
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="1"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>